<commit_message>
add a new line
</commit_message>
<xml_diff>
--- a/ONBW Mass creation _OIN.xlsx
+++ b/ONBW Mass creation _OIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binko.xie\Desktop\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9537082D-B244-4212-971F-537C766B0FBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550A60E7-338C-49D2-807B-5983B5D393C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="651" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="185">
   <si>
     <t>Material</t>
   </si>
@@ -612,19 +612,29 @@
   </si>
   <si>
     <t>P14230012316</t>
+  </si>
+  <si>
+    <t>P14230012317</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -727,11 +737,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -746,22 +756,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -776,19 +786,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -1079,7 +1090,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
+      <selection pane="bottomRight" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3003,7 +3014,9 @@
       <c r="L54"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55"/>
+      <c r="A55" s="24" t="s">
+        <v>184</v>
+      </c>
       <c r="F55"/>
       <c r="G55"/>
       <c r="H55"/>

</xml_diff>